<commit_message>
update call node url
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="login" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="posttext" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="searchrepository" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="posttext" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,21 +13,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>url</t>
-  </si>
-  <si>
     <t>content</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>pass</t>
+    <t>repository name</t>
+  </si>
+  <si>
+    <t>CrossBrowser</t>
   </si>
   <si>
     <t>hello</t>
@@ -35,13 +42,13 @@
     <t>nice to meet you</t>
   </si>
   <si>
-    <t>https://www.facebook.com</t>
+    <t>https://github.com/login</t>
   </si>
   <si>
     <t>maihoathaoit@gmail.com</t>
   </si>
   <si>
-    <t>SaiGon2019</t>
+    <t>Xanh$&amp;@Ngoc654</t>
   </si>
 </sst>
 </file>
@@ -100,6 +107,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -112,24 +123,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -152,10 +163,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
@@ -163,7 +174,38 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -171,7 +213,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>